<commit_message>
actualizacion de la doc (falta riesgos)
</commit_message>
<xml_diff>
--- a/Documentos/Planilla de cambios (6+1 Software).xlsx
+++ b/Documentos/Planilla de cambios (6+1 Software).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AEB333-09AA-437A-BD7C-28F3AAD5334B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9388FA02-8F7E-4569-AC18-2C100DA36AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1A86829-FAC1-44C0-BD05-C13760C68DBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Fecha aparición</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>Se creara un sistema de reportes con su menu propio y ahi estaran los reportes que le usuario quiera ver, en este caso se mostrara la cantidad de visitanes que autentico el usuario</t>
+  </si>
+  <si>
+    <t>Configuraciones</t>
+  </si>
+  <si>
+    <t>Ampliar la idea de configuraciones del sistema donde en vez de solo tener una opcion que sea cambiar el ruteo de conexion se tengan otras opciones adicionales</t>
+  </si>
+  <si>
+    <t>Darle al usuario mas libertad de personalizacion del sistema</t>
+  </si>
+  <si>
+    <t>Se tendra que ampliar la ventana de configuraciones creando las mismas y las funcionalidades correspondientes a cada opcion</t>
   </si>
 </sst>
 </file>
@@ -201,15 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -535,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009CB019-81E1-470F-8A22-04EB59761B8C}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,131 +592,116 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="82.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>45412</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>45415</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>45420</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="82.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>45426</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>45428</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="5">
+        <v>45440</v>
+      </c>
     </row>
     <row r="6" spans="2:10" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>45426</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>45428</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+    <row r="7" spans="2:10" ht="72" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>45440</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45444</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>